<commit_message>
correcao do orcamento faltando aparte de vacalo
</commit_message>
<xml_diff>
--- a/PastaDocumentos/orcamento.xlsx
+++ b/PastaDocumentos/orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Downloads\ExercicioGit\3SIPF-ExemploGIT-2024\PastaDocumentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E730D5C7-4675-47CF-838B-EDC20AAD227B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CFB052-58B3-4E41-ABC5-829D47B2CA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Orçamento</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>valor Mensal</t>
+  </si>
+  <si>
+    <t>cavalo</t>
+  </si>
+  <si>
+    <t>vacalo</t>
   </si>
 </sst>
 </file>
@@ -51,7 +57,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_([$BRL]\ * #,##0.00_);_([$BRL]\ * \(#,##0.00\);_([$BRL]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$BRL]\ * #,##0.00_);_([$BRL]\ * \(#,##0.00\);_([$BRL]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -90,9 +96,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -374,24 +381,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -399,7 +407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -407,7 +415,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -415,12 +423,28 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>12000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2">
+        <v>85200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>